<commit_message>
Actualizacion lista herramientas innovacion'
</commit_message>
<xml_diff>
--- a/necessity_artifact/data/lista_innovacion.xlsx
+++ b/necessity_artifact/data/lista_innovacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/OneDrive - Grupo Bancolombia/innovation-platform/necessity_artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F906C944-AF4B-3F49-A3F9-BA92F27ACB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705198DB-9B1E-B94B-A721-D58E7DB315ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{A39C73BE-FBB6-E74C-9DA2-9FDCB2429089}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{A39C73BE-FBB6-E74C-9DA2-9FDCB2429089}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2108,7 +2108,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2122,7 +2122,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2310,7 +2310,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3378,7 +3378,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3656,7 +3656,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3670,7 +3670,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3684,7 +3684,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3834,7 +3834,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3848,7 +3848,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3862,7 +3862,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3876,7 +3876,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3890,7 +3890,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3904,7 +3904,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -3918,7 +3918,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4054,7 +4054,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4063,7 +4063,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4134,7 +4134,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4148,7 +4148,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4298,7 +4298,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4312,7 +4312,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4340,7 +4340,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4368,7 +4368,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4574,7 +4574,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -4790,7 +4790,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5108,7 +5108,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5320,7 +5320,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5329,7 +5329,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5344,7 +5344,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5353,7 +5353,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -5532,7 +5532,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -7541,6 +7541,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7555,10 +7559,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7878,8 +7878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5230DFF3-271F-374E-9956-6AFBF4B421FD}">
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7895,25 +7895,25 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="29" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
@@ -8544,7 +8544,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J11" s="16">
         <v>0.5</v>
@@ -9077,7 +9077,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I19" s="16">
         <v>0</v>
@@ -9089,7 +9089,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M19" s="17">
         <v>3</v>
@@ -10599,7 +10599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6688077D-3B9A-574C-9D2E-D9052A08F2FF}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
@@ -10613,25 +10613,25 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="29" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
     </row>
     <row r="2" spans="1:22" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -12304,16 +12304,16 @@
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="26" t="s">
         <v>460</v>
       </c>
-      <c r="H28" s="32" t="s">
+      <c r="H28" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="I28" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="J28" s="32" t="s">
+      <c r="J28" s="27" t="s">
         <v>463</v>
       </c>
     </row>

</xml_diff>